<commit_message>
Fix article in output file
</commit_message>
<xml_diff>
--- a/Excel/Bailey/15.02.2022 Bailey — техничка part1.xlsx
+++ b/Excel/Bailey/15.02.2022 Bailey — техничка part1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Bailey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB262CD5-AB1A-4AF8-96E2-D91B245C92A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A9B9D0-8FF9-48DD-9BBE-DDBB20296B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DF93E06-745E-43BB-B362-39D65D7A1090}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8FB4635-C7F6-4857-BA01-37FF7860FF43}"/>
   </bookViews>
   <sheets>
     <sheet name="Техничка Bailey" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
     <t>Natural/Black</t>
   </si>
   <si>
-    <t>new</t>
+    <t>21-782-26</t>
   </si>
   <si>
     <t>22805BH</t>
@@ -1224,7 +1224,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0402AF58-C329-4997-AAE3-3BECE782AB08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09DA48EC-D24D-49CD-95C8-1726883DD8D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1274,7 +1274,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{519BBC8C-1048-4250-8287-616F5FE5B9E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871D1ED3-5EE3-4A35-AF42-4BCEE78F7DCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,7 +1324,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEDF3EA5-D2CC-4848-B052-EFE795165CB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CCA4519-7901-4DDD-8F9B-E7D46B054C8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,7 +1374,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7CE1331-78AD-4987-B858-5B07B4C88CC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE98698-5641-4FCC-B8BC-6670A29F3B62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1424,7 @@
         <xdr:cNvPr id="6" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790BBC95-D530-4A7C-BB43-CDB0EB498DFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2463CC48-E748-4AC0-B19B-EBB971ADFF71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1474,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AABAD9C-F8AE-406A-955D-DFCD79236DE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B483096-9788-4F46-B665-10B46BA0023A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1524,7 +1524,7 @@
         <xdr:cNvPr id="8" name="Рисунок 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F3CA65-EC80-4012-BAF9-F7CA3D7DDAF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAAAF914-6BC2-4704-96DA-F6BD111E0A4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1574,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD1B23A-D8EC-4FEE-BC39-56CF52D9137F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA67315B-62E7-45B9-9EEA-45D3FED5EE76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="10" name="Рисунок 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19FA8EE0-E668-4B81-AE59-8781FBCB7CF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368517A7-3036-40E3-A087-73C6EC646926}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,7 +1674,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B59E2FD8-F5B5-4544-9064-00CD90A0F8F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963B6DC6-8463-46CA-A8BD-F7B018C15262}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1724,7 +1724,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE5E782-38AB-4B64-91DC-A4EF2C5A4B65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCCC829-9697-48E5-B85A-05630E4766CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1774,7 +1774,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{304B76E2-EBA9-4EAD-B26D-C29F13B15F6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{324B93DD-F12B-4865-8CCB-2E3C8B8AC3BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1824,7 +1824,7 @@
         <xdr:cNvPr id="14" name="Рисунок 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{206CF6AE-7E0C-4F49-BEA5-7720769E9753}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8531B8F-661F-448F-A688-E969B53C49BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1874,7 +1874,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1709F2EB-5E89-433C-9FC6-3A19DF85A7A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9747C4BC-6E03-488C-A023-3C6974B4B406}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1924,7 @@
         <xdr:cNvPr id="16" name="Рисунок 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C3F7BDF-7FA9-4FE2-AAB3-676E5A690947}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E01E38-943D-4A09-82A7-FE83353F830D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,7 +1974,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFB9940B-A2CB-478F-887F-871BFD90B10C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78FD4D7-8E28-44DB-B3EC-E59B7097AAD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2024,7 +2024,7 @@
         <xdr:cNvPr id="18" name="Рисунок 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A006EECD-9282-4635-81EA-465D050AD089}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7320AAB-F03A-4535-A6FB-8F2EAB66B85A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2074,7 +2074,7 @@
         <xdr:cNvPr id="19" name="Рисунок 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D3E2B0-89E7-4165-A714-25692B3A338D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D9CCB6-57F3-4BC9-AFAB-05F2185747D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2124,7 +2124,7 @@
         <xdr:cNvPr id="20" name="Рисунок 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97D23D32-FFBC-4939-8335-C982177E2B55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A2C7664-24DA-475F-9C0D-D052B0D5B5EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2174,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA0AB05-F44E-43FE-B842-629BEB79A216}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FF509F-219D-49FA-A263-7DD92435692F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2224,7 +2224,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1B7C0B6-A325-431F-914C-21174DAE7B5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB22CAC-5194-45E8-B548-DBE470EFB07A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2274,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13541AFA-B743-4C8F-B9A8-62CF7916B055}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA26D004-D5EC-4AE2-9CBD-92D08E3EA4DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2324,7 +2324,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E1E7FB-D073-4830-82C3-64F52CCFDC65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86991688-7926-4380-BB36-B4A290E7AB92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2374,7 +2374,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CCE903A-3803-4ADE-89A8-BCA5FF8FB5EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB0511E-5537-488F-AF46-E1F42DF2F964}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2424,7 +2424,7 @@
         <xdr:cNvPr id="26" name="Рисунок 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB531EA-9B0B-49B0-B3CF-64E71C00C87D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C858829-B9FC-4DF4-A721-378C502698A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2474,7 +2474,7 @@
         <xdr:cNvPr id="27" name="Рисунок 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB3905C-14C3-49CA-B1D4-7BD62D0A2435}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C261FC4-0ACB-4C70-98AA-98411D41E0EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2524,7 +2524,7 @@
         <xdr:cNvPr id="28" name="Рисунок 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CF0299E-3C1F-469B-8123-3AED4FE1F42C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{092DAA28-8771-4654-93E9-B1E27A62CEC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2574,7 +2574,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C5F1CE-19CD-459C-9D23-8AAFC54219B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6933AD-3422-4AA0-9995-BC27748C0B2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2624,7 +2624,7 @@
         <xdr:cNvPr id="30" name="Рисунок 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4032AEE0-D04C-4552-BCB8-DF1E5178F7A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B88532D-2AF5-4AF4-A8B2-DBD93F6306DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2674,7 +2674,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E87063A-77E4-4771-AD07-200D90EA5A8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E2897E-40C0-4B5B-9601-F123B4697F2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2724,7 +2724,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6E8980C-5654-49AB-B608-311E6AF4EEEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191A5289-433C-4069-9E1D-7FF998B13605}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,7 +2774,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C2C897-EAA7-4F98-BC5C-CD3A1969E5EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A2526D7-25DD-4290-8A63-A85FFA8EEA86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2824,7 +2824,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E467F0CB-0749-456D-9F0C-7132B9D2A341}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B45A1F-304A-4727-9502-E443190C00B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2874,7 +2874,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7D62A65-FBDE-496F-8F2C-0000AEC4A47E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CF9C81-7DF7-4800-89BB-AD988DE8B5B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2924,7 +2924,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA0DE25-9885-4C74-A3CE-A4500F71515C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79931ECF-6908-47EF-8B03-EBFB55BAEAC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2974,7 +2974,7 @@
         <xdr:cNvPr id="37" name="Рисунок 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B2FD622-E5AC-42CA-9723-FFABE40707AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8238A726-4765-4EB7-9C94-6E973B497059}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3024,7 +3024,7 @@
         <xdr:cNvPr id="38" name="Рисунок 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1A51022-F135-4D42-8EFA-73757F09D3F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450598DB-0341-4437-8F22-B70BF772F503}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3074,7 +3074,7 @@
         <xdr:cNvPr id="39" name="Рисунок 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5D2CA2D-CFB4-4C03-924D-AAC748FEB016}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF75D14-297C-41DA-9A71-2078515FB476}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3124,7 +3124,7 @@
         <xdr:cNvPr id="40" name="Рисунок 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB085F15-96DE-42B6-AFF4-F45C4916E65D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE1DB38-99F4-4484-A738-1791B9157749}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3174,7 +3174,7 @@
         <xdr:cNvPr id="41" name="Рисунок 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F69D93AE-A5FA-4470-8641-DF9AC53A567C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B2602CB-3ED7-4663-9ABB-7A856C68E01D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3224,7 +3224,7 @@
         <xdr:cNvPr id="42" name="Рисунок 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA40D93-2020-4F27-8035-E15BB206AA3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DEF18BB-4CB7-4860-BAC7-C2D0FA02517F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3274,7 +3274,7 @@
         <xdr:cNvPr id="43" name="Рисунок 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C7049A-3149-4322-A10D-7A62F430FC9D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D9A37D-E850-42ED-BFB7-1B7428CB5039}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3324,7 +3324,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A7A966-A506-4859-B807-587A45CE549E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5151E6-F0D8-4B28-895C-8ED1ED93968C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3374,7 +3374,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9F02014-FB35-4A6C-AA01-FB2AEDA60CB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B74C490F-DE4A-4C0C-88DE-691EEBD3635E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3424,7 +3424,7 @@
         <xdr:cNvPr id="46" name="Рисунок 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE41515B-73B9-4E40-8D93-4F6744BF0BAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BD5472-9C64-4682-BCD5-DEB1F01FBC26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3474,7 +3474,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9FB637E-D68B-4133-BEB8-596D69E74239}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4593599B-B529-4316-870E-84F8F8934A04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3524,7 +3524,7 @@
         <xdr:cNvPr id="48" name="Рисунок 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5150229B-8887-446C-8663-4F0CC2E2BBBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FAE7649-ED49-431B-966D-59847CFECE64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3574,7 +3574,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FF0B5F-B07D-4E5F-84C5-DAA9472BD5D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA99E206-47FA-4EF1-8C57-56BB22BF5337}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3624,7 +3624,7 @@
         <xdr:cNvPr id="50" name="Рисунок 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{452976A3-AC46-489B-930E-845E22143918}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E323929-B7F6-44E3-8949-40622F2D36A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3674,7 +3674,7 @@
         <xdr:cNvPr id="51" name="Рисунок 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FFE0449-D35B-4F7A-838B-7F052AE4BC6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1DF82B-EEB7-453F-BF5D-27E84F67C0D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3724,7 +3724,7 @@
         <xdr:cNvPr id="52" name="Рисунок 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{684B61EC-8E44-4B6D-B484-C0063898A143}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D2FAC6-BC64-44B0-834C-96AFE094B303}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3774,7 +3774,7 @@
         <xdr:cNvPr id="53" name="Рисунок 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A682FF91-8228-43DF-BA2D-533C8614BFEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C5133C-5D84-4BCA-BF58-FBB11ECC74E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3824,7 +3824,7 @@
         <xdr:cNvPr id="54" name="Рисунок 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693A38B4-18F5-4E0B-9A73-1A58A10F32FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F9C00E2-680D-4D6C-9801-5A7FFBEF6F23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3874,7 +3874,7 @@
         <xdr:cNvPr id="55" name="Рисунок 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EBA0B29-5A69-4400-9609-08EB019C9EE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A88FCCF-B2EE-42A0-8D1B-055EE0F1147C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3924,7 +3924,7 @@
         <xdr:cNvPr id="56" name="Рисунок 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20CD79B-0428-4390-856A-289BA58626D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D87C70-7DE5-426D-8F41-4A02CCA63794}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3974,7 +3974,7 @@
         <xdr:cNvPr id="57" name="Рисунок 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA11497A-E9E6-4A9B-801E-284A52D4D901}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA960FC-772B-40C9-8382-7DD7E2BD163D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4024,7 +4024,7 @@
         <xdr:cNvPr id="58" name="Рисунок 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC17A92-BA00-420C-9081-E4796B25B04A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{724545E7-323F-4F3E-B78B-4DCDF54BFC15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4074,7 +4074,7 @@
         <xdr:cNvPr id="59" name="Рисунок 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3DF3AB5-9219-4EEB-B00E-0C926078543A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1819253D-A7DA-4644-8E04-C16C1F780A78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4124,7 +4124,7 @@
         <xdr:cNvPr id="60" name="Рисунок 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AD9AA0-C2D0-4594-BEF4-CA23EE62A2D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB7DC8A-F6FC-4A45-A1F8-905809DB1143}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4174,7 +4174,7 @@
         <xdr:cNvPr id="61" name="Рисунок 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52E504D3-9D1D-49F3-BC5F-73ECCA4FF2C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA79C896-7C17-451A-B1C5-1CA50C9D2254}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4224,7 +4224,7 @@
         <xdr:cNvPr id="62" name="Рисунок 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66BEFE3-8E9A-4166-AEAE-2FE215A42432}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F299E7-385F-4C51-9716-75B032B76641}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4274,7 +4274,7 @@
         <xdr:cNvPr id="63" name="Рисунок 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4CF5357-9DCB-42D9-9519-73E8DBB0E247}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC82914-A573-4FD0-90D7-D11D706FD9B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4324,7 +4324,7 @@
         <xdr:cNvPr id="64" name="Рисунок 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A57B021D-DB03-4966-97F2-6DEEA0A69FB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3BF9ED9-FDE6-4440-AE47-FF9F08928918}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4374,7 +4374,7 @@
         <xdr:cNvPr id="65" name="Рисунок 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E7FB0B-B74C-4C0F-A149-A14F0F7BD205}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243AEFF8-7242-4DCD-A4F7-88388844DC83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4424,7 +4424,7 @@
         <xdr:cNvPr id="66" name="Рисунок 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8A81B77-A1D9-42D5-A017-5E0A87DEEB7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95BBDB58-A619-430D-8D81-908779FF5D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
         <xdr:cNvPr id="67" name="Рисунок 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E6355F-44B4-413F-A2ED-DE57F0552204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E77D8BD-AA98-4A23-87FB-5BFBFAFE3994}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4524,7 +4524,7 @@
         <xdr:cNvPr id="68" name="Рисунок 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C93096F-A07B-4E56-A9A8-C8DAA63E16A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F6F56B-62FA-4FFA-BE9B-D9253B967FDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4574,7 +4574,7 @@
         <xdr:cNvPr id="69" name="Рисунок 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49272BF3-48BE-41D3-BF66-4AF10BB1054E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA7F3DDD-59BF-443E-B7D9-10213E91F360}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4624,7 +4624,7 @@
         <xdr:cNvPr id="70" name="Рисунок 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{754EB4CA-0D06-43FD-A3F6-E245C444FDAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A85DAEE5-32A3-4FBC-84BC-5D1A788E6037}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4674,7 +4674,7 @@
         <xdr:cNvPr id="71" name="Рисунок 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A0BA684-0559-48F9-BD10-99D494670882}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D0D4A84-9CB2-43C5-95E6-C3E31E999517}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4724,7 +4724,7 @@
         <xdr:cNvPr id="72" name="Рисунок 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131B44C5-DF38-40FE-8F66-17C0CBC7D0E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{212D779C-ABCA-482B-83D1-37481780C6C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4774,7 +4774,7 @@
         <xdr:cNvPr id="73" name="Рисунок 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A185AA3D-909E-434C-848E-89E49A07242C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F97B1B42-EDC6-4015-9B3B-653CE8A50560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4824,7 +4824,7 @@
         <xdr:cNvPr id="74" name="Рисунок 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22F74228-043D-49FC-9052-C6085746D36E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5462A4-CACC-4F7D-AE65-F4C37D506DA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4874,7 +4874,7 @@
         <xdr:cNvPr id="75" name="Рисунок 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155843D3-6806-4B28-A75E-A865DC737857}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B549BFE9-1D91-433B-BFC3-DB6320EE45DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4924,7 +4924,7 @@
         <xdr:cNvPr id="76" name="Рисунок 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04831583-3703-4A99-8FB8-E3A3662985B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B21301B5-FEE9-4465-AFB1-EF713A5D8FE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4974,7 +4974,7 @@
         <xdr:cNvPr id="77" name="Рисунок 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E856FB7-A769-47DD-9D48-FBE1ED572904}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14144B1-A945-43BF-B34B-7ECDAC505809}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5024,7 +5024,7 @@
         <xdr:cNvPr id="78" name="Рисунок 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84570051-CD25-4779-A06E-8DAD7EF00CF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51DC62FA-EB91-4ADD-92D0-DADD94927F46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5074,7 +5074,7 @@
         <xdr:cNvPr id="79" name="Рисунок 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{997459EF-A54F-4314-BFC7-9CF6D600B09B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C75F088-01AF-4DA9-837E-7E85E0BD09CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5124,7 +5124,7 @@
         <xdr:cNvPr id="80" name="Рисунок 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2C0A60-818C-44D3-8CCE-3A85EFB7AB08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95D56DB0-18AD-4F94-98DA-45D82E7A4A8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5174,7 +5174,7 @@
         <xdr:cNvPr id="81" name="Рисунок 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABCC982A-54BA-4611-9969-336333732C0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D217942E-3371-4EE0-84AA-3DDEFF688ED0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5224,7 +5224,7 @@
         <xdr:cNvPr id="82" name="Рисунок 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85927BDE-505A-49F0-94E1-84EC57277BB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E507BC0-86AC-46A8-AEDB-7948F0D0129B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5555,14 +5555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440382DE-E5DC-4FE2-AE40-87476ACB3EE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FAAF43-C363-4A21-B405-BFBC9CD8E626}">
   <sheetPr codeName="Лист9">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:BD153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>
@@ -15012,7 +15012,7 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:AM1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AM82" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Rebase output file (153 row)
</commit_message>
<xml_diff>
--- a/Excel/Bailey/15.02.2022 Bailey — техничка part1.xlsx
+++ b/Excel/Bailey/15.02.2022 Bailey — техничка part1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Bailey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A9B9D0-8FF9-48DD-9BBE-DDBB20296B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3858A3CC-D371-4066-AE3E-4E69B8496F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8FB4635-C7F6-4857-BA01-37FF7860FF43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90D5BD8C-9C0E-4689-82DB-CE7506F51FFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Техничка Bailey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="292">
   <si>
     <t>Артикул на этикетке</t>
   </si>
@@ -910,27 +910,6 @@
   </si>
   <si>
     <t>21-755-08</t>
-  </si>
-  <si>
-    <t>21-253-14</t>
-  </si>
-  <si>
-    <t>25102 TAXTEN</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Требуется код страны</t>
-  </si>
-  <si>
-    <t>Требуются кол-во и нетто</t>
-  </si>
-  <si>
-    <t>Требуются кол-во и брутто</t>
-  </si>
-  <si>
-    <t>Требуются кол-во и цена</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1183,10 +1162,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1224,7 +1199,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09DA48EC-D24D-49CD-95C8-1726883DD8D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDFC6375-FCD6-49EC-BDBE-825D3D7CA3FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1274,7 +1249,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871D1ED3-5EE3-4A35-AF42-4BCEE78F7DCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94F41397-F23F-429A-86DA-C05B23D0FC8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,7 +1299,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CCA4519-7901-4DDD-8F9B-E7D46B054C8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16F5E795-072E-48D0-9351-4600300B8E52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,7 +1349,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE98698-5641-4FCC-B8BC-6670A29F3B62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01976179-ABC3-4D73-AA8D-3E657CCFF4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1399,7 @@
         <xdr:cNvPr id="6" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2463CC48-E748-4AC0-B19B-EBB971ADFF71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{656A4E01-E19C-42AE-A558-B6B1E7E645F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1449,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B483096-9788-4F46-B665-10B46BA0023A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A9A47B6-5DB0-4640-8FF0-3F6872E6174E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1524,7 +1499,7 @@
         <xdr:cNvPr id="8" name="Рисунок 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAAAF914-6BC2-4704-96DA-F6BD111E0A4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39F74B19-FCC0-427D-B7CC-1B8B3F392CF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1549,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA67315B-62E7-45B9-9EEA-45D3FED5EE76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BED8E308-912D-43EF-97B9-95912B5D6243}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1624,7 +1599,7 @@
         <xdr:cNvPr id="10" name="Рисунок 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368517A7-3036-40E3-A087-73C6EC646926}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84A289E-1D7C-4015-B067-65D5B7E27D26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,7 +1649,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963B6DC6-8463-46CA-A8BD-F7B018C15262}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5554F7F-9AA2-48FA-A9C8-4A2B1B9088E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1724,7 +1699,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCCC829-9697-48E5-B85A-05630E4766CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DD21D9C-7001-423B-83C0-1552B2B5B34D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1774,7 +1749,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{324B93DD-F12B-4865-8CCB-2E3C8B8AC3BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F447D26-8A9B-459D-8CEE-53E687DBC055}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1824,7 +1799,7 @@
         <xdr:cNvPr id="14" name="Рисунок 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8531B8F-661F-448F-A688-E969B53C49BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDFAFDD6-8E0D-4933-9537-C448E6F20EB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1874,7 +1849,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9747C4BC-6E03-488C-A023-3C6974B4B406}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121D0E9E-377B-4A96-BEFA-E3A98BDA21FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1899,7 @@
         <xdr:cNvPr id="16" name="Рисунок 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E01E38-943D-4A09-82A7-FE83353F830D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{940F7DDC-911F-483E-8637-BD20CE65B874}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,7 +1949,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78FD4D7-8E28-44DB-B3EC-E59B7097AAD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B499191B-153B-407D-BF60-9267CC545835}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2024,7 +1999,7 @@
         <xdr:cNvPr id="18" name="Рисунок 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7320AAB-F03A-4535-A6FB-8F2EAB66B85A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83A61017-6D2D-49CC-8C31-08E9644E965E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2074,7 +2049,7 @@
         <xdr:cNvPr id="19" name="Рисунок 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D9CCB6-57F3-4BC9-AFAB-05F2185747D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03F748E7-9255-450A-AEB8-1A45C9C5FCC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2124,7 +2099,7 @@
         <xdr:cNvPr id="20" name="Рисунок 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A2C7664-24DA-475F-9C0D-D052B0D5B5EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F6E6C7D-137B-49E9-963A-DD1B35F4947E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2149,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FF509F-219D-49FA-A263-7DD92435692F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E02AD66F-A637-4CD5-90FE-E26579F799F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2224,7 +2199,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB22CAC-5194-45E8-B548-DBE470EFB07A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93034228-1304-4D55-A6BF-49B648B0A4AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2249,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA26D004-D5EC-4AE2-9CBD-92D08E3EA4DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711A8346-011D-438E-AEA1-1A13FBAA6051}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2324,7 +2299,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86991688-7926-4380-BB36-B4A290E7AB92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8039598B-0CCD-4B32-943B-81BA51D97A01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2374,7 +2349,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB0511E-5537-488F-AF46-E1F42DF2F964}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6D2357-F68D-4848-A090-13E43BC01240}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2424,7 +2399,7 @@
         <xdr:cNvPr id="26" name="Рисунок 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C858829-B9FC-4DF4-A721-378C502698A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5587D843-0CF9-4B15-AB3C-AAAE94BD7C49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2474,7 +2449,7 @@
         <xdr:cNvPr id="27" name="Рисунок 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C261FC4-0ACB-4C70-98AA-98411D41E0EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1427B331-46BA-40CF-B316-0EB37AF5EB8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2524,7 +2499,7 @@
         <xdr:cNvPr id="28" name="Рисунок 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{092DAA28-8771-4654-93E9-B1E27A62CEC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E05077FA-D136-4736-99E4-82BA6E2B042E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2574,7 +2549,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6933AD-3422-4AA0-9995-BC27748C0B2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AAA23E-1C0D-46AE-A622-49C9906553B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2624,7 +2599,7 @@
         <xdr:cNvPr id="30" name="Рисунок 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B88532D-2AF5-4AF4-A8B2-DBD93F6306DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702DEE3F-26BC-4C27-992C-3B2B2F1667D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2674,7 +2649,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E2897E-40C0-4B5B-9601-F123B4697F2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281D4E3C-19A5-4710-9280-0EFC92B72AB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2724,7 +2699,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191A5289-433C-4069-9E1D-7FF998B13605}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB5DEDA7-476A-4800-A4CB-FFE12DEB2C31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,7 +2749,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A2526D7-25DD-4290-8A63-A85FFA8EEA86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC6634AC-5C13-413C-81DA-D39AC3B56165}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2824,7 +2799,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B45A1F-304A-4727-9502-E443190C00B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7E55C3-E452-48CF-9276-53A67EFC8F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2874,7 +2849,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CF9C81-7DF7-4800-89BB-AD988DE8B5B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36A6C951-8215-4E7B-AF3C-608C6147A3A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2924,7 +2899,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79931ECF-6908-47EF-8B03-EBFB55BAEAC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6A4421-FA70-4264-97D8-8E3FB335339F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2974,7 +2949,7 @@
         <xdr:cNvPr id="37" name="Рисунок 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8238A726-4765-4EB7-9C94-6E973B497059}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB421C91-4153-4E7B-96A8-754A7D8B7CDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3024,7 +2999,7 @@
         <xdr:cNvPr id="38" name="Рисунок 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450598DB-0341-4437-8F22-B70BF772F503}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE874132-8F4D-46EC-9CF4-713AB1627E73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3074,7 +3049,7 @@
         <xdr:cNvPr id="39" name="Рисунок 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF75D14-297C-41DA-9A71-2078515FB476}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB53593-6E3C-452E-96EA-7670ABF275CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3124,7 +3099,7 @@
         <xdr:cNvPr id="40" name="Рисунок 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE1DB38-99F4-4484-A738-1791B9157749}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E74FCDE-C3F8-4666-B58D-D84684BB75EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3174,7 +3149,7 @@
         <xdr:cNvPr id="41" name="Рисунок 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B2602CB-3ED7-4663-9ABB-7A856C68E01D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E66D6E9D-3E1F-49CC-BF83-D50EA96C99D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3224,7 +3199,7 @@
         <xdr:cNvPr id="42" name="Рисунок 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DEF18BB-4CB7-4860-BAC7-C2D0FA02517F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57B5A3F4-FB1B-4BFB-93F6-520AF16897F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3274,7 +3249,7 @@
         <xdr:cNvPr id="43" name="Рисунок 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D9A37D-E850-42ED-BFB7-1B7428CB5039}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{215B9564-9BA7-4855-8774-2421D90D8C1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3324,7 +3299,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5151E6-F0D8-4B28-895C-8ED1ED93968C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB71F2DA-6AA2-4700-A513-626D9FA707D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3374,7 +3349,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B74C490F-DE4A-4C0C-88DE-691EEBD3635E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFF1BC20-3BD3-41E3-9283-194E2F5CF7BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3424,7 +3399,7 @@
         <xdr:cNvPr id="46" name="Рисунок 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BD5472-9C64-4682-BCD5-DEB1F01FBC26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1403F62-05A0-4B62-AF6A-D9ED8C6BAD6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3474,7 +3449,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4593599B-B529-4316-870E-84F8F8934A04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D77C9FD3-2684-466A-9F33-1F032AFB0E4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3524,7 +3499,7 @@
         <xdr:cNvPr id="48" name="Рисунок 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FAE7649-ED49-431B-966D-59847CFECE64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0B6718A-C1C3-46D6-9580-5C5410B3458C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3574,7 +3549,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA99E206-47FA-4EF1-8C57-56BB22BF5337}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D34CD1DF-4A82-47F8-B366-81B0F62C9EA7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3624,7 +3599,7 @@
         <xdr:cNvPr id="50" name="Рисунок 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E323929-B7F6-44E3-8949-40622F2D36A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAAEF0C6-CAD0-4A49-A7F9-43F7A66C5441}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3674,7 +3649,7 @@
         <xdr:cNvPr id="51" name="Рисунок 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1DF82B-EEB7-453F-BF5D-27E84F67C0D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A2938C-9BAC-42E7-8601-BD7F69813D48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3724,7 +3699,7 @@
         <xdr:cNvPr id="52" name="Рисунок 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D2FAC6-BC64-44B0-834C-96AFE094B303}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7DE55C-03D8-445C-936B-434CC22FE524}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3774,7 +3749,7 @@
         <xdr:cNvPr id="53" name="Рисунок 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C5133C-5D84-4BCA-BF58-FBB11ECC74E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3210FFF-6F96-41CE-892B-E1572EB42250}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3824,7 +3799,7 @@
         <xdr:cNvPr id="54" name="Рисунок 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F9C00E2-680D-4D6C-9801-5A7FFBEF6F23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C15CB6F1-6D64-440B-B5E8-E7F2C9C49553}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3874,7 +3849,7 @@
         <xdr:cNvPr id="55" name="Рисунок 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A88FCCF-B2EE-42A0-8D1B-055EE0F1147C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B69472D-33B2-444C-9429-0C3082E54BEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3924,7 +3899,7 @@
         <xdr:cNvPr id="56" name="Рисунок 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D87C70-7DE5-426D-8F41-4A02CCA63794}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855C4400-3692-47A7-971D-617906D0E7B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3974,7 +3949,7 @@
         <xdr:cNvPr id="57" name="Рисунок 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA960FC-772B-40C9-8382-7DD7E2BD163D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A73A589-D5BE-424F-BFEA-AF2E9B00F565}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4024,7 +3999,7 @@
         <xdr:cNvPr id="58" name="Рисунок 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{724545E7-323F-4F3E-B78B-4DCDF54BFC15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD257688-7904-4AB9-8439-9760C7100CDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4074,7 +4049,7 @@
         <xdr:cNvPr id="59" name="Рисунок 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1819253D-A7DA-4644-8E04-C16C1F780A78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E428612-D343-4AEF-B8C3-A3F259DBC5D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4124,7 +4099,7 @@
         <xdr:cNvPr id="60" name="Рисунок 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB7DC8A-F6FC-4A45-A1F8-905809DB1143}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED311D22-1461-4AC1-BA6F-D82C85C6625C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4174,7 +4149,7 @@
         <xdr:cNvPr id="61" name="Рисунок 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA79C896-7C17-451A-B1C5-1CA50C9D2254}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37375989-CF6F-4791-8662-1D793555C171}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4224,7 +4199,7 @@
         <xdr:cNvPr id="62" name="Рисунок 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F299E7-385F-4C51-9716-75B032B76641}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978EB3F7-C10B-42FC-94F8-11979A09DE78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4274,7 +4249,7 @@
         <xdr:cNvPr id="63" name="Рисунок 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC82914-A573-4FD0-90D7-D11D706FD9B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380FC2F0-AE48-4ED2-8422-F5AA29DA90A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4324,7 +4299,7 @@
         <xdr:cNvPr id="64" name="Рисунок 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3BF9ED9-FDE6-4440-AE47-FF9F08928918}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3538DA9D-3B62-4508-BC09-655552BAD417}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4374,7 +4349,7 @@
         <xdr:cNvPr id="65" name="Рисунок 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243AEFF8-7242-4DCD-A4F7-88388844DC83}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2C2FE56-2F98-41F3-8CD2-AAC9181AF6EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4424,7 +4399,7 @@
         <xdr:cNvPr id="66" name="Рисунок 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95BBDB58-A619-430D-8D81-908779FF5D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46141C16-8336-4AA4-AEB1-9B9BC863AD7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4449,7 @@
         <xdr:cNvPr id="67" name="Рисунок 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E77D8BD-AA98-4A23-87FB-5BFBFAFE3994}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00CFB040-6F51-4D66-A1B1-35204E1A5535}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4524,7 +4499,7 @@
         <xdr:cNvPr id="68" name="Рисунок 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F6F56B-62FA-4FFA-BE9B-D9253B967FDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{400C061B-B5A0-4B08-918D-EAEB9F723CE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4574,7 +4549,7 @@
         <xdr:cNvPr id="69" name="Рисунок 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA7F3DDD-59BF-443E-B7D9-10213E91F360}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F4B974D-695E-4B17-A529-CB0E3645CCAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4624,7 +4599,7 @@
         <xdr:cNvPr id="70" name="Рисунок 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A85DAEE5-32A3-4FBC-84BC-5D1A788E6037}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE66E7C7-D542-4AB4-A6EC-D76A8CAA115C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4674,7 +4649,7 @@
         <xdr:cNvPr id="71" name="Рисунок 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D0D4A84-9CB2-43C5-95E6-C3E31E999517}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7151D6-5ED9-4505-B9EC-8C057C708E83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4724,7 +4699,7 @@
         <xdr:cNvPr id="72" name="Рисунок 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{212D779C-ABCA-482B-83D1-37481780C6C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E03F664-5759-4154-8800-C916B8320EC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4774,7 +4749,7 @@
         <xdr:cNvPr id="73" name="Рисунок 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F97B1B42-EDC6-4015-9B3B-653CE8A50560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B04E1C2-3216-4B0E-A0E4-105DD6EC354F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4824,7 +4799,7 @@
         <xdr:cNvPr id="74" name="Рисунок 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5462A4-CACC-4F7D-AE65-F4C37D506DA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE2F020-0011-4B38-9C5F-65A40BF5C64C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4874,7 +4849,7 @@
         <xdr:cNvPr id="75" name="Рисунок 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B549BFE9-1D91-433B-BFC3-DB6320EE45DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB4D5BBB-1AD4-40CC-8E6F-2E2FF46D4C62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4924,7 +4899,7 @@
         <xdr:cNvPr id="76" name="Рисунок 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B21301B5-FEE9-4465-AFB1-EF713A5D8FE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610C416F-6B11-44C8-944E-E4388B59A3E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4974,7 +4949,7 @@
         <xdr:cNvPr id="77" name="Рисунок 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14144B1-A945-43BF-B34B-7ECDAC505809}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94A50CE1-7121-4BD5-95DA-953B92728B7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5024,7 +4999,7 @@
         <xdr:cNvPr id="78" name="Рисунок 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51DC62FA-EB91-4ADD-92D0-DADD94927F46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{728A9004-C34C-46EC-921E-51ACD63FC586}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5074,7 +5049,7 @@
         <xdr:cNvPr id="79" name="Рисунок 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C75F088-01AF-4DA9-837E-7E85E0BD09CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{323F8B6F-B0F5-4030-A412-1C487A3D9A41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5124,7 +5099,7 @@
         <xdr:cNvPr id="80" name="Рисунок 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95D56DB0-18AD-4F94-98DA-45D82E7A4A8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{342287AC-2B41-4612-A2BC-2F2F44EF5FE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5174,7 +5149,7 @@
         <xdr:cNvPr id="81" name="Рисунок 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D217942E-3371-4EE0-84AA-3DDEFF688ED0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C348A1B-FED8-4457-9B14-157CF897633E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5224,7 +5199,7 @@
         <xdr:cNvPr id="82" name="Рисунок 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E507BC0-86AC-46A8-AEDB-7948F0D0129B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26757312-95A2-48A7-BCC7-28C93E3FD384}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5555,14 +5530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FAAF43-C363-4A21-B405-BFBC9CD8E626}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB74121-840B-4A28-BCFA-F1CFB71FD823}">
   <sheetPr codeName="Лист9">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:BD153"/>
+  <dimension ref="A1:BD152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>
@@ -14955,61 +14930,6 @@
       <c r="AL152" s="34"/>
       <c r="AM152" s="35"/>
     </row>
-    <row r="153" spans="1:39" s="26" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="B153" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="D153" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E153" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F153" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G153" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I153" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="J153" s="30" t="s">
-        <v>290</v>
-      </c>
-      <c r="K153" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="L153" s="30"/>
-      <c r="AD153" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF153" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="AG153" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="AH153" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="AI153" s="23">
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="AJ153" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="AK153" s="23" t="s">
-        <v>297</v>
-      </c>
-      <c r="AL153" s="34"/>
-      <c r="AM153" s="37" t="s">
-        <v>298</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:AM82" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>